<commit_message>
changes to planting randomization to include front and writing proposal
</commit_message>
<xml_diff>
--- a/growing_conditions/PlantingData.xlsx
+++ b/growing_conditions/PlantingData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moin2\OneDrive\Documents\Horsenettle\growing_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6217203-FB5D-4A3E-A489-F8C9B1BC7D5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59481F4F-3436-46B4-8BE1-007986F2E559}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFAFF3EB-B419-47E1-98F1-7FCFAB378E2D}"/>
   </bookViews>
@@ -578,7 +578,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,9 +654,7 @@
       <c r="I2" s="1">
         <v>44253</v>
       </c>
-      <c r="J2" s="1">
-        <v>44254</v>
-      </c>
+      <c r="J2" s="1"/>
       <c r="K2" s="1">
         <v>44254</v>
       </c>
@@ -686,9 +684,7 @@
       <c r="I3" s="1">
         <v>44253</v>
       </c>
-      <c r="J3" s="1">
-        <v>44254</v>
-      </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="1">
         <v>44254</v>
       </c>
@@ -718,9 +714,7 @@
       <c r="I4" s="1">
         <v>44253</v>
       </c>
-      <c r="J4" s="1">
-        <v>44254</v>
-      </c>
+      <c r="J4" s="1"/>
       <c r="K4" s="1">
         <v>44254</v>
       </c>
@@ -750,10 +744,10 @@
       <c r="I5" s="1">
         <v>44253</v>
       </c>
-      <c r="J5" s="1">
-        <v>44254</v>
-      </c>
-      <c r="K5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1">
+        <v>44260</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -780,9 +774,7 @@
       <c r="I6" s="1">
         <v>44253</v>
       </c>
-      <c r="J6" s="1">
-        <v>44254</v>
-      </c>
+      <c r="J6" s="1"/>
       <c r="K6" s="1">
         <v>44254</v>
       </c>
@@ -809,6 +801,13 @@
       <c r="G7" s="1">
         <v>44187</v>
       </c>
+      <c r="I7" s="1">
+        <v>44260</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1">
+        <v>44260</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -832,6 +831,9 @@
       <c r="G8" s="1">
         <v>44187</v>
       </c>
+      <c r="I8" s="1">
+        <v>44260</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -855,6 +857,12 @@
       <c r="G9" s="1">
         <v>44187</v>
       </c>
+      <c r="I9" s="1">
+        <v>44260</v>
+      </c>
+      <c r="K9" s="1">
+        <v>44260</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -878,6 +886,12 @@
       <c r="G10" s="1">
         <v>44187</v>
       </c>
+      <c r="I10" s="1">
+        <v>44260</v>
+      </c>
+      <c r="K10" s="1">
+        <v>44260</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -900,6 +914,12 @@
       </c>
       <c r="G11" s="1">
         <v>44187</v>
+      </c>
+      <c r="I11" s="1">
+        <v>44260</v>
+      </c>
+      <c r="K11" s="1">
+        <v>44260</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated horsenettle plant info
</commit_message>
<xml_diff>
--- a/growing_conditions/PlantingData.xlsx
+++ b/growing_conditions/PlantingData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moin2\OneDrive\Documents\Horsenettle\growing_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59481F4F-3436-46B4-8BE1-007986F2E559}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9097B6C-6B48-4924-BAF2-8F6DAD70D9B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFAFF3EB-B419-47E1-98F1-7FCFAB378E2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="69">
   <si>
     <t>Ramet</t>
   </si>
@@ -223,6 +223,24 @@
   </si>
   <si>
     <t>photosynthesis</t>
+  </si>
+  <si>
+    <t>FR8</t>
+  </si>
+  <si>
+    <t>FR11</t>
+  </si>
+  <si>
+    <t>FR6</t>
+  </si>
+  <si>
+    <t>FR10</t>
+  </si>
+  <si>
+    <t>FR1</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -575,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C2BDB9-DDA1-4456-B96B-B7C6BC14A59C}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,7 +850,10 @@
         <v>44187</v>
       </c>
       <c r="I8" s="1">
-        <v>44260</v>
+        <v>44295</v>
+      </c>
+      <c r="K8" s="1">
+        <v>44282</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -944,6 +965,12 @@
       <c r="G12" s="1">
         <v>44211</v>
       </c>
+      <c r="I12" s="1">
+        <v>44282</v>
+      </c>
+      <c r="K12" s="1">
+        <v>44282</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -967,6 +994,12 @@
       <c r="G13" s="1">
         <v>44211</v>
       </c>
+      <c r="I13" s="1">
+        <v>44282</v>
+      </c>
+      <c r="K13" s="1">
+        <v>44282</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -990,6 +1023,12 @@
       <c r="G14" s="1">
         <v>44211</v>
       </c>
+      <c r="I14" s="1">
+        <v>44282</v>
+      </c>
+      <c r="K14" s="1">
+        <v>44282</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1013,6 +1052,12 @@
       <c r="G15" s="1">
         <v>44211</v>
       </c>
+      <c r="I15" s="1">
+        <v>44282</v>
+      </c>
+      <c r="K15" s="1">
+        <v>44282</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1036,8 +1081,14 @@
       <c r="G16" s="1">
         <v>44211</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I16" s="1">
+        <v>44282</v>
+      </c>
+      <c r="K16" s="1">
+        <v>44282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1059,8 +1110,14 @@
       <c r="G17" s="1">
         <v>44218</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I17" s="1">
+        <v>44289</v>
+      </c>
+      <c r="K17" s="1">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1082,8 +1139,14 @@
       <c r="G18" s="1">
         <v>44218</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I18" s="1">
+        <v>44289</v>
+      </c>
+      <c r="K18" s="1">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1105,8 +1168,14 @@
       <c r="G19" s="1">
         <v>44218</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I19" s="1">
+        <v>44289</v>
+      </c>
+      <c r="K19" s="1">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1128,8 +1197,14 @@
       <c r="G20" s="1">
         <v>44218</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I20" s="1">
+        <v>44289</v>
+      </c>
+      <c r="K20" s="1">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1151,8 +1226,14 @@
       <c r="G21" s="1">
         <v>44218</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I21" s="1">
+        <v>44289</v>
+      </c>
+      <c r="K21" s="1">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1174,8 +1255,14 @@
       <c r="G22" s="1">
         <v>44218</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I22" s="1">
+        <v>44289</v>
+      </c>
+      <c r="K22" s="1">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1185,6 +1272,9 @@
       <c r="C23">
         <v>22</v>
       </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
       <c r="E23" t="s">
         <v>51</v>
       </c>
@@ -1192,10 +1282,10 @@
         <v>15</v>
       </c>
       <c r="G23" s="1">
-        <v>44226</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1205,17 +1295,20 @@
       <c r="C24">
         <v>23</v>
       </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
       <c r="E24" t="s">
         <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G24" s="1">
-        <v>44226</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1225,17 +1318,20 @@
       <c r="C25">
         <v>24</v>
       </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
       <c r="E25" t="s">
         <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G25" s="1">
-        <v>44226</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1245,17 +1341,20 @@
       <c r="C26">
         <v>25</v>
       </c>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
       <c r="E26" t="s">
         <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G26" s="1">
-        <v>44226</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1265,17 +1364,20 @@
       <c r="C27">
         <v>26</v>
       </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
       <c r="E27" t="s">
         <v>55</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G27" s="1">
-        <v>44226</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1297,8 +1399,14 @@
       <c r="G28" s="1">
         <v>44236</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I28" s="1">
+        <v>44295</v>
+      </c>
+      <c r="K28" s="1">
+        <v>44295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1320,8 +1428,14 @@
       <c r="G29" s="1">
         <v>44236</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I29" s="1">
+        <v>44295</v>
+      </c>
+      <c r="K29" s="1">
+        <v>44295</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1344,7 +1458,7 @@
         <v>44236</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1367,7 +1481,7 @@
         <v>44236</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -1389,8 +1503,14 @@
       <c r="G32" s="1">
         <v>44236</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I32" s="1">
+        <v>44295</v>
+      </c>
+      <c r="K32" s="1">
+        <v>44295</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -1404,7 +1524,7 @@
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
@@ -1412,8 +1532,17 @@
       <c r="G33" s="1">
         <v>44246</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="1">
+        <v>44297</v>
+      </c>
+      <c r="I33" s="1">
+        <v>44301</v>
+      </c>
+      <c r="K33" s="1">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -1424,7 +1553,7 @@
         <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1435,8 +1564,17 @@
       <c r="G34" s="1">
         <v>44246</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="1">
+        <v>44297</v>
+      </c>
+      <c r="I34" s="1">
+        <v>44301</v>
+      </c>
+      <c r="K34" s="1">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1450,7 +1588,7 @@
         <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F35" t="s">
         <v>10</v>
@@ -1458,8 +1596,14 @@
       <c r="G35" s="1">
         <v>44246</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I35" s="1">
+        <v>44301</v>
+      </c>
+      <c r="K35" s="1">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -1481,8 +1625,14 @@
       <c r="G36" s="1">
         <v>44246</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I36" s="1">
+        <v>44301</v>
+      </c>
+      <c r="K36" s="1">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -1493,7 +1643,7 @@
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E37" t="s">
         <v>52</v>
@@ -1504,8 +1654,14 @@
       <c r="G37" s="1">
         <v>44246</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I37" s="1">
+        <v>44301</v>
+      </c>
+      <c r="K37" s="1">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -1528,7 +1684,7 @@
         <v>44253</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -1551,7 +1707,7 @@
         <v>44253</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -1574,7 +1730,7 @@
         <v>44253</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -1597,7 +1753,7 @@
         <v>44253</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -1618,6 +1774,704 @@
       </c>
       <c r="G42" s="1">
         <v>44253</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>42</v>
+      </c>
+      <c r="D43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" t="s">
+        <v>51</v>
+      </c>
+      <c r="F43" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="1">
+        <v>44267</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>43</v>
+      </c>
+      <c r="D44" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="1">
+        <v>44267</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45">
+        <v>44</v>
+      </c>
+      <c r="D45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" s="1">
+        <v>44267</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>45</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="1">
+        <v>44267</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <v>9</v>
+      </c>
+      <c r="C47">
+        <v>46</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" s="1">
+        <v>44267</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48" s="1">
+        <v>44274</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>48</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="1">
+        <v>44274</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>49</v>
+      </c>
+      <c r="D50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" s="1">
+        <v>44274</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>50</v>
+      </c>
+      <c r="D51" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" t="s">
+        <v>55</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" s="1">
+        <v>44274</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52">
+        <v>10</v>
+      </c>
+      <c r="C52">
+        <v>51</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" s="1">
+        <v>44274</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>52</v>
+      </c>
+      <c r="D53" t="s">
+        <v>64</v>
+      </c>
+      <c r="E53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="1">
+        <v>44274</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54">
+        <v>11</v>
+      </c>
+      <c r="C54">
+        <v>53</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
+        <v>28</v>
+      </c>
+      <c r="F54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="1">
+        <v>44282</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55">
+        <v>11</v>
+      </c>
+      <c r="C55">
+        <v>54</v>
+      </c>
+      <c r="D55" t="s">
+        <v>47</v>
+      </c>
+      <c r="E55" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="1">
+        <v>44282</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56">
+        <v>11</v>
+      </c>
+      <c r="C56">
+        <v>55</v>
+      </c>
+      <c r="D56" t="s">
+        <v>37</v>
+      </c>
+      <c r="E56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="1">
+        <v>44282</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <v>56</v>
+      </c>
+      <c r="D57" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="1">
+        <v>44282</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58">
+        <v>11</v>
+      </c>
+      <c r="C58">
+        <v>57</v>
+      </c>
+      <c r="D58" t="s">
+        <v>45</v>
+      </c>
+      <c r="E58" t="s">
+        <v>34</v>
+      </c>
+      <c r="F58" t="s">
+        <v>15</v>
+      </c>
+      <c r="G58" s="1">
+        <v>44282</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59">
+        <v>12</v>
+      </c>
+      <c r="C59">
+        <v>58</v>
+      </c>
+      <c r="D59" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59" t="s">
+        <v>21</v>
+      </c>
+      <c r="F59" t="s">
+        <v>15</v>
+      </c>
+      <c r="G59" s="1">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60">
+        <v>12</v>
+      </c>
+      <c r="C60">
+        <v>59</v>
+      </c>
+      <c r="D60" t="s">
+        <v>31</v>
+      </c>
+      <c r="E60" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" t="s">
+        <v>15</v>
+      </c>
+      <c r="G60" s="1">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61">
+        <v>12</v>
+      </c>
+      <c r="C61">
+        <v>60</v>
+      </c>
+      <c r="D61" t="s">
+        <v>43</v>
+      </c>
+      <c r="E61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" t="s">
+        <v>15</v>
+      </c>
+      <c r="G61" s="1">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62">
+        <v>12</v>
+      </c>
+      <c r="C62">
+        <v>61</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="1">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63">
+        <v>12</v>
+      </c>
+      <c r="C63">
+        <v>62</v>
+      </c>
+      <c r="D63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" t="s">
+        <v>55</v>
+      </c>
+      <c r="F63" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" s="1">
+        <v>44288</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64">
+        <v>13</v>
+      </c>
+      <c r="C64">
+        <v>63</v>
+      </c>
+      <c r="D64" t="s">
+        <v>66</v>
+      </c>
+      <c r="E64" t="s">
+        <v>54</v>
+      </c>
+      <c r="F64" t="s">
+        <v>15</v>
+      </c>
+      <c r="G64" s="1">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65">
+        <v>13</v>
+      </c>
+      <c r="C65">
+        <v>64</v>
+      </c>
+      <c r="D65" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" t="s">
+        <v>48</v>
+      </c>
+      <c r="F65" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" s="1">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66">
+        <v>13</v>
+      </c>
+      <c r="C66">
+        <v>65</v>
+      </c>
+      <c r="D66" t="s">
+        <v>35</v>
+      </c>
+      <c r="E66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F66" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="1">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67">
+        <v>13</v>
+      </c>
+      <c r="C67">
+        <v>66</v>
+      </c>
+      <c r="D67" t="s">
+        <v>24</v>
+      </c>
+      <c r="E67" t="s">
+        <v>32</v>
+      </c>
+      <c r="F67" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" s="1">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68">
+        <v>13</v>
+      </c>
+      <c r="C68">
+        <v>67</v>
+      </c>
+      <c r="D68" t="s">
+        <v>33</v>
+      </c>
+      <c r="E68" t="s">
+        <v>27</v>
+      </c>
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68" s="1">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>14</v>
+      </c>
+      <c r="C69">
+        <v>68</v>
+      </c>
+      <c r="D69" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" t="s">
+        <v>46</v>
+      </c>
+      <c r="F69" t="s">
+        <v>15</v>
+      </c>
+      <c r="G69" s="1">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>14</v>
+      </c>
+      <c r="C70">
+        <v>69</v>
+      </c>
+      <c r="D70" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" t="s">
+        <v>53</v>
+      </c>
+      <c r="F70" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="1">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>14</v>
+      </c>
+      <c r="C71">
+        <v>70</v>
+      </c>
+      <c r="D71" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" t="s">
+        <v>36</v>
+      </c>
+      <c r="F71" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" s="1">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>14</v>
+      </c>
+      <c r="C72">
+        <v>71</v>
+      </c>
+      <c r="D72" t="s">
+        <v>49</v>
+      </c>
+      <c r="E72" t="s">
+        <v>44</v>
+      </c>
+      <c r="F72" t="s">
+        <v>15</v>
+      </c>
+      <c r="G72" s="1">
+        <v>44301</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>14</v>
+      </c>
+      <c r="C73">
+        <v>72</v>
+      </c>
+      <c r="D73" t="s">
+        <v>63</v>
+      </c>
+      <c r="E73" t="s">
+        <v>51</v>
+      </c>
+      <c r="F73" t="s">
+        <v>10</v>
+      </c>
+      <c r="G73" s="1">
+        <v>44301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inputting CMS, chlorophyll, planting, and flowering data
</commit_message>
<xml_diff>
--- a/growing_conditions/PlantingData.xlsx
+++ b/growing_conditions/PlantingData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moin2\OneDrive\Documents\Horsenettle\growing_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9097B6C-6B48-4924-BAF2-8F6DAD70D9B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B3D0C-FC5B-4D89-B270-FAFA8DAD70A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFAFF3EB-B419-47E1-98F1-7FCFAB378E2D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="71">
   <si>
     <t>Ramet</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>chlorophyll_cold</t>
   </si>
 </sst>
 </file>
@@ -593,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C2BDB9-DDA1-4456-B96B-B7C6BC14A59C}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:M89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+      <selection activeCell="A23" sqref="A23:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,9 +610,10 @@
     <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -641,10 +648,13 @@
         <v>61</v>
       </c>
       <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -672,12 +682,15 @@
       <c r="I2" s="1">
         <v>44253</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1">
+        <v>44309</v>
+      </c>
       <c r="K2" s="1">
         <v>44254</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -702,12 +715,15 @@
       <c r="I3" s="1">
         <v>44253</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1">
+        <v>44309</v>
+      </c>
       <c r="K3" s="1">
         <v>44254</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -732,12 +748,15 @@
       <c r="I4" s="1">
         <v>44253</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1">
+        <v>44309</v>
+      </c>
       <c r="K4" s="1">
         <v>44254</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -762,12 +781,15 @@
       <c r="I5" s="1">
         <v>44253</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1">
+        <v>44309</v>
+      </c>
       <c r="K5" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -792,12 +814,15 @@
       <c r="I6" s="1">
         <v>44253</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1">
+        <v>44309</v>
+      </c>
       <c r="K6" s="1">
         <v>44254</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -822,12 +847,15 @@
       <c r="I7" s="1">
         <v>44260</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <v>44316</v>
+      </c>
       <c r="K7" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -852,11 +880,15 @@
       <c r="I8" s="1">
         <v>44295</v>
       </c>
+      <c r="J8" s="1">
+        <v>44316</v>
+      </c>
       <c r="K8" s="1">
         <v>44282</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -881,11 +913,15 @@
       <c r="I9" s="1">
         <v>44260</v>
       </c>
+      <c r="J9" s="1">
+        <v>44316</v>
+      </c>
       <c r="K9" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -910,11 +946,15 @@
       <c r="I10" s="1">
         <v>44260</v>
       </c>
+      <c r="J10" s="1">
+        <v>44316</v>
+      </c>
       <c r="K10" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -939,11 +979,15 @@
       <c r="I11" s="1">
         <v>44260</v>
       </c>
+      <c r="J11" s="1">
+        <v>44316</v>
+      </c>
       <c r="K11" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -968,11 +1012,15 @@
       <c r="I12" s="1">
         <v>44282</v>
       </c>
+      <c r="J12" s="1">
+        <v>44323</v>
+      </c>
       <c r="K12" s="1">
         <v>44282</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -997,11 +1045,15 @@
       <c r="I13" s="1">
         <v>44282</v>
       </c>
+      <c r="J13" s="1">
+        <v>44323</v>
+      </c>
       <c r="K13" s="1">
         <v>44282</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1026,11 +1078,15 @@
       <c r="I14" s="1">
         <v>44282</v>
       </c>
+      <c r="J14" s="1">
+        <v>44323</v>
+      </c>
       <c r="K14" s="1">
         <v>44282</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1055,11 +1111,15 @@
       <c r="I15" s="1">
         <v>44282</v>
       </c>
+      <c r="J15" s="1">
+        <v>44323</v>
+      </c>
       <c r="K15" s="1">
         <v>44282</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1084,11 +1144,15 @@
       <c r="I16" s="1">
         <v>44282</v>
       </c>
+      <c r="J16" s="1">
+        <v>44323</v>
+      </c>
       <c r="K16" s="1">
         <v>44282</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1116,8 +1180,9 @@
       <c r="K17" s="1">
         <v>44289</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1145,8 +1210,9 @@
       <c r="K18" s="1">
         <v>44289</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1174,8 +1240,9 @@
       <c r="K19" s="1">
         <v>44289</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1203,8 +1270,9 @@
       <c r="K20" s="1">
         <v>44289</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1232,8 +1300,9 @@
       <c r="K21" s="1">
         <v>44289</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1261,8 +1330,9 @@
       <c r="K22" s="1">
         <v>44289</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1284,8 +1354,15 @@
       <c r="G23" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I23" s="1">
+        <v>44316</v>
+      </c>
+      <c r="K23" s="1">
+        <v>44315</v>
+      </c>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1307,8 +1384,15 @@
       <c r="G24" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I24" s="1">
+        <v>44316</v>
+      </c>
+      <c r="K24" s="1">
+        <v>44315</v>
+      </c>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1330,8 +1414,15 @@
       <c r="G25" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I25" s="1">
+        <v>44316</v>
+      </c>
+      <c r="K25" s="1">
+        <v>44315</v>
+      </c>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1353,8 +1444,15 @@
       <c r="G26" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I26" s="1">
+        <v>44316</v>
+      </c>
+      <c r="K26" s="1">
+        <v>44315</v>
+      </c>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1376,8 +1474,15 @@
       <c r="G27" s="1">
         <v>44260</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I27" s="1">
+        <v>44316</v>
+      </c>
+      <c r="K27" s="1">
+        <v>44315</v>
+      </c>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1405,8 +1510,9 @@
       <c r="K28" s="1">
         <v>44295</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1434,8 +1540,9 @@
       <c r="K29" s="1">
         <v>44295</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1458,7 +1565,7 @@
         <v>44236</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1481,7 +1588,7 @@
         <v>44236</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -1509,8 +1616,9 @@
       <c r="K32" s="1">
         <v>44295</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -1541,8 +1649,9 @@
       <c r="K33" s="1">
         <v>44301</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -1573,8 +1682,9 @@
       <c r="K34" s="1">
         <v>44301</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1602,8 +1712,9 @@
       <c r="K35" s="1">
         <v>44301</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -1631,8 +1742,9 @@
       <c r="K36" s="1">
         <v>44301</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -1660,8 +1772,9 @@
       <c r="K37" s="1">
         <v>44301</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -1683,8 +1796,15 @@
       <c r="G38" s="1">
         <v>44253</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I38" s="1">
+        <v>44309</v>
+      </c>
+      <c r="K38" s="1">
+        <v>44309</v>
+      </c>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -1706,8 +1826,15 @@
       <c r="G39" s="1">
         <v>44253</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I39" s="1">
+        <v>44309</v>
+      </c>
+      <c r="K39" s="1">
+        <v>44309</v>
+      </c>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -1729,8 +1856,15 @@
       <c r="G40" s="1">
         <v>44253</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I40" s="1">
+        <v>44309</v>
+      </c>
+      <c r="K40" s="1">
+        <v>44309</v>
+      </c>
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -1752,8 +1886,15 @@
       <c r="G41" s="1">
         <v>44253</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I41" s="1">
+        <v>44309</v>
+      </c>
+      <c r="K41" s="1">
+        <v>44309</v>
+      </c>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -1775,8 +1916,15 @@
       <c r="G42" s="1">
         <v>44253</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I42" s="1">
+        <v>44309</v>
+      </c>
+      <c r="K42" s="1">
+        <v>44309</v>
+      </c>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1798,8 +1946,10 @@
       <c r="G43" s="1">
         <v>44267</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -1821,8 +1971,10 @@
       <c r="G44" s="1">
         <v>44267</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -1845,7 +1997,7 @@
         <v>44267</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -1868,7 +2020,7 @@
         <v>44267</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -1891,7 +2043,7 @@
         <v>44267</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1913,8 +2065,15 @@
       <c r="G48" s="1">
         <v>44274</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I48" s="1">
+        <v>44323</v>
+      </c>
+      <c r="K48" s="1">
+        <v>44325</v>
+      </c>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -1936,8 +2095,15 @@
       <c r="G49" s="1">
         <v>44274</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I49" s="1">
+        <v>44323</v>
+      </c>
+      <c r="K49" s="1">
+        <v>44325</v>
+      </c>
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -1959,8 +2125,15 @@
       <c r="G50" s="1">
         <v>44274</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I50" s="1">
+        <v>44323</v>
+      </c>
+      <c r="K50" s="1">
+        <v>44325</v>
+      </c>
+      <c r="L50" s="1"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1982,8 +2155,15 @@
       <c r="G51" s="1">
         <v>44274</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I51" s="1">
+        <v>44323</v>
+      </c>
+      <c r="K51" s="1">
+        <v>44325</v>
+      </c>
+      <c r="L51" s="1"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1997,7 +2177,7 @@
         <v>13</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F52" t="s">
         <v>10</v>
@@ -2005,8 +2185,18 @@
       <c r="G52" s="1">
         <v>44274</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52" s="1">
+        <v>44322</v>
+      </c>
+      <c r="I52" s="1">
+        <v>44323</v>
+      </c>
+      <c r="K52" s="1">
+        <v>44325</v>
+      </c>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2020,7 +2210,7 @@
         <v>64</v>
       </c>
       <c r="E53" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
@@ -2028,8 +2218,9 @@
       <c r="G53" s="1">
         <v>44274</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -2052,7 +2243,7 @@
         <v>44282</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -2075,7 +2266,7 @@
         <v>44282</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -2098,7 +2289,7 @@
         <v>44282</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -2121,7 +2312,7 @@
         <v>44282</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -2144,7 +2335,7 @@
         <v>44282</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -2167,7 +2358,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -2190,7 +2381,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -2213,7 +2404,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -2236,7 +2427,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -2259,7 +2450,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -2375,6 +2566,9 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
       <c r="B69">
         <v>14</v>
       </c>
@@ -2395,6 +2589,9 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>68</v>
+      </c>
       <c r="B70">
         <v>14</v>
       </c>
@@ -2415,6 +2612,9 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>68</v>
+      </c>
       <c r="B71">
         <v>14</v>
       </c>
@@ -2435,6 +2635,9 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>68</v>
+      </c>
       <c r="B72">
         <v>14</v>
       </c>
@@ -2455,6 +2658,9 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>68</v>
+      </c>
       <c r="B73">
         <v>14</v>
       </c>
@@ -2472,6 +2678,374 @@
       </c>
       <c r="G73" s="1">
         <v>44301</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74">
+        <v>15</v>
+      </c>
+      <c r="C74">
+        <v>73</v>
+      </c>
+      <c r="D74" t="s">
+        <v>41</v>
+      </c>
+      <c r="E74" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74" s="1">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>68</v>
+      </c>
+      <c r="B75">
+        <v>15</v>
+      </c>
+      <c r="C75">
+        <v>74</v>
+      </c>
+      <c r="D75" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" t="s">
+        <v>19</v>
+      </c>
+      <c r="F75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75" s="1">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76">
+        <v>15</v>
+      </c>
+      <c r="C76">
+        <v>75</v>
+      </c>
+      <c r="D76" t="s">
+        <v>67</v>
+      </c>
+      <c r="E76" t="s">
+        <v>40</v>
+      </c>
+      <c r="F76" t="s">
+        <v>15</v>
+      </c>
+      <c r="G76" s="1">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77">
+        <v>15</v>
+      </c>
+      <c r="C77">
+        <v>76</v>
+      </c>
+      <c r="D77" t="s">
+        <v>39</v>
+      </c>
+      <c r="E77" t="s">
+        <v>30</v>
+      </c>
+      <c r="F77" t="s">
+        <v>10</v>
+      </c>
+      <c r="G77" s="1">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78">
+        <v>15</v>
+      </c>
+      <c r="C78">
+        <v>77</v>
+      </c>
+      <c r="D78" t="s">
+        <v>57</v>
+      </c>
+      <c r="E78" t="s">
+        <v>42</v>
+      </c>
+      <c r="F78" t="s">
+        <v>10</v>
+      </c>
+      <c r="G78" s="1">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79">
+        <v>15</v>
+      </c>
+      <c r="C79">
+        <v>78</v>
+      </c>
+      <c r="D79" t="s">
+        <v>65</v>
+      </c>
+      <c r="E79" t="s">
+        <v>23</v>
+      </c>
+      <c r="F79" t="s">
+        <v>10</v>
+      </c>
+      <c r="G79" s="1">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>69</v>
+      </c>
+      <c r="B80">
+        <v>16</v>
+      </c>
+      <c r="C80">
+        <v>79</v>
+      </c>
+      <c r="D80" t="s">
+        <v>35</v>
+      </c>
+      <c r="E80" t="s">
+        <v>16</v>
+      </c>
+      <c r="F80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G80" s="1">
+        <v>44315</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81">
+        <v>16</v>
+      </c>
+      <c r="C81">
+        <v>80</v>
+      </c>
+      <c r="D81" t="s">
+        <v>37</v>
+      </c>
+      <c r="E81" t="s">
+        <v>52</v>
+      </c>
+      <c r="F81" t="s">
+        <v>15</v>
+      </c>
+      <c r="G81" s="1">
+        <v>44315</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>69</v>
+      </c>
+      <c r="B82">
+        <v>16</v>
+      </c>
+      <c r="C82">
+        <v>81</v>
+      </c>
+      <c r="D82" t="s">
+        <v>67</v>
+      </c>
+      <c r="E82" t="s">
+        <v>40</v>
+      </c>
+      <c r="F82" t="s">
+        <v>15</v>
+      </c>
+      <c r="G82" s="1">
+        <v>44315</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>69</v>
+      </c>
+      <c r="B83">
+        <v>16</v>
+      </c>
+      <c r="C83">
+        <v>82</v>
+      </c>
+      <c r="D83" t="s">
+        <v>18</v>
+      </c>
+      <c r="E83" t="s">
+        <v>23</v>
+      </c>
+      <c r="F83" t="s">
+        <v>10</v>
+      </c>
+      <c r="G83" s="1">
+        <v>44315</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84">
+        <v>16</v>
+      </c>
+      <c r="C84">
+        <v>83</v>
+      </c>
+      <c r="D84" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" t="s">
+        <v>28</v>
+      </c>
+      <c r="F84" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84" s="1">
+        <v>44315</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85">
+        <v>17</v>
+      </c>
+      <c r="C85">
+        <v>84</v>
+      </c>
+      <c r="D85" t="s">
+        <v>43</v>
+      </c>
+      <c r="E85" t="s">
+        <v>36</v>
+      </c>
+      <c r="F85" t="s">
+        <v>15</v>
+      </c>
+      <c r="G85" s="1">
+        <v>44322</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>69</v>
+      </c>
+      <c r="B86">
+        <v>17</v>
+      </c>
+      <c r="C86">
+        <v>85</v>
+      </c>
+      <c r="D86" t="s">
+        <v>41</v>
+      </c>
+      <c r="E86" t="s">
+        <v>48</v>
+      </c>
+      <c r="F86" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86" s="1">
+        <v>44322</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87">
+        <v>17</v>
+      </c>
+      <c r="C87">
+        <v>86</v>
+      </c>
+      <c r="D87" t="s">
+        <v>20</v>
+      </c>
+      <c r="E87" t="s">
+        <v>30</v>
+      </c>
+      <c r="F87" t="s">
+        <v>15</v>
+      </c>
+      <c r="G87" s="1">
+        <v>44322</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>69</v>
+      </c>
+      <c r="B88">
+        <v>17</v>
+      </c>
+      <c r="C88">
+        <v>87</v>
+      </c>
+      <c r="D88" t="s">
+        <v>24</v>
+      </c>
+      <c r="E88" t="s">
+        <v>44</v>
+      </c>
+      <c r="F88" t="s">
+        <v>10</v>
+      </c>
+      <c r="G88" s="1">
+        <v>44322</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89">
+        <v>17</v>
+      </c>
+      <c r="C89">
+        <v>88</v>
+      </c>
+      <c r="D89" t="s">
+        <v>17</v>
+      </c>
+      <c r="E89" t="s">
+        <v>38</v>
+      </c>
+      <c r="F89" t="s">
+        <v>10</v>
+      </c>
+      <c r="G89" s="1">
+        <v>44322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>